<commit_message>
Update 2p0. Convention change to support multi-axle vehicles
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Aero/sm_car_data_Aero_Coefficients.xlsx
+++ b/Libraries/Vehicle/Aero/sm_car_data_Aero_Coefficients.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Vehicle\Aero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAA5347-FE59-424A-BEB8-867C077C9B64}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B0A88F-9C68-47FC-9D98-587AB11B6F38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="10152" tabRatio="648" activeTab="3" xr2:uid="{F771CC24-0E19-4696-9A47-DE53EE9C34AF}"/>
+    <workbookView xWindow="960" yWindow="900" windowWidth="17280" windowHeight="10215" tabRatio="760" firstSheet="1" activeTab="6" xr2:uid="{F771CC24-0E19-4696-9A47-DE53EE9C34AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sedan_HambaLG" sheetId="1" r:id="rId1"/>
     <sheet name="Sedan_Hamba" sheetId="2" r:id="rId2"/>
     <sheet name="Bus_Makhulu" sheetId="3" r:id="rId3"/>
-    <sheet name="Trailer_Elula" sheetId="4" r:id="rId4"/>
-    <sheet name="Trailer_Thwala" sheetId="5" r:id="rId5"/>
+    <sheet name="Truck_Amandla" sheetId="6" r:id="rId4"/>
+    <sheet name="Trailer_Elula" sheetId="4" r:id="rId5"/>
+    <sheet name="Trailer_Thwala" sheetId="5" r:id="rId6"/>
+    <sheet name="Trailer_Kumanzi" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="27">
   <si>
     <t>Units</t>
   </si>
@@ -110,6 +112,12 @@
   </si>
   <si>
     <t>Trailer_Thwala</t>
+  </si>
+  <si>
+    <t>Truck_Amandla</t>
+  </si>
+  <si>
+    <t>Trailer_Kumanzi</t>
   </si>
 </sst>
 </file>
@@ -1037,13 +1045,183 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E120840-12C0-4B7A-802E-95D96C22C3B1}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E9" sqref="E9"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5:H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="8" width="10" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14">
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="15">
+        <v>-1.2</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EDBA4F-1D14-46EF-A741-9E01D906A994}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
@@ -1206,7 +1384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD17D0A8-637E-4354-8C2C-BAF4E2145F01}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
@@ -1374,4 +1552,174 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7292BC-C2AF-4E54-A4E0-99355D0A6C5B}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E9" sqref="E9"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="8" width="10" customWidth="1"/>
+    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14">
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="15">
+        <v>5</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v2.6 Added decoupled suspension, four-wheel steering, scripts to generate GGV diagram
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Aero/sm_car_data_Aero_Coefficients.xlsx
+++ b/Libraries/Vehicle/Aero/sm_car_data_Aero_Coefficients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Vehicle\Aero\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Aero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B0A88F-9C68-47FC-9D98-587AB11B6F38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FECDE37-2355-42EC-81FD-EEAC9C194360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="900" windowWidth="17280" windowHeight="10215" tabRatio="760" firstSheet="1" activeTab="6" xr2:uid="{F771CC24-0E19-4696-9A47-DE53EE9C34AF}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" tabRatio="760" activeTab="1" xr2:uid="{F771CC24-0E19-4696-9A47-DE53EE9C34AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sedan_HambaLG" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Trailer_Elula" sheetId="4" r:id="rId5"/>
     <sheet name="Trailer_Thwala" sheetId="5" r:id="rId6"/>
     <sheet name="Trailer_Kumanzi" sheetId="7" r:id="rId7"/>
+    <sheet name="FSAE_Achilles" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="28">
   <si>
     <t>Units</t>
   </si>
@@ -118,6 +119,9 @@
   </si>
   <si>
     <t>Trailer_Kumanzi</t>
+  </si>
+  <si>
+    <t>FSAE_Achilles</t>
   </si>
 </sst>
 </file>
@@ -546,21 +550,21 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -580,7 +584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -594,7 +598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -608,7 +612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -622,7 +626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -637,7 +641,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -649,7 +653,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -664,7 +668,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -679,7 +683,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -711,26 +715,26 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -750,7 +754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -764,7 +768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -778,7 +782,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -792,7 +796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -807,7 +811,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -819,7 +823,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -834,7 +838,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -845,11 +849,11 @@
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="15">
-        <v>2.81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="14">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -889,18 +893,18 @@
       <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -920,7 +924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -934,7 +938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -948,7 +952,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -962,7 +966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -977,7 +981,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -989,7 +993,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1019,7 +1023,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1059,18 +1063,18 @@
       <selection pane="bottomRight" activeCell="H5" sqref="H5:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1090,7 +1094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1104,7 +1108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1132,7 +1136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1151,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1159,7 +1163,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1189,7 +1193,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1229,18 +1233,18 @@
       <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1260,7 +1264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1274,7 +1278,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1288,7 +1292,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1302,7 +1306,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1317,7 +1321,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1329,7 +1333,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1344,7 +1348,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1359,7 +1363,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1399,18 +1403,18 @@
       <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1430,7 +1434,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1444,7 +1448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1458,7 +1462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1472,7 +1476,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1487,7 +1491,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1499,7 +1503,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1514,7 +1518,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1529,7 +1533,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1561,7 +1565,7 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
@@ -1569,18 +1573,18 @@
       <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1600,7 +1604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1614,7 +1618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1628,7 +1632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -1642,7 +1646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1657,7 +1661,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1669,7 +1673,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1684,7 +1688,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1699,7 +1703,7 @@
         <v>2.81</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1716,6 +1720,176 @@
       </c>
       <c r="H9" s="15">
         <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D7273B-0F4A-4F6A-A593-DC5540A6D580}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="E9" sqref="E9"/>
+      <selection pane="topRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="10" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14">
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="15">
+        <v>-0.8</v>
+      </c>
+      <c r="G9" s="15">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v3p0 Major file cleanup
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Aero/sm_car_data_Aero_Coefficients.xlsx
+++ b/Libraries/Vehicle/Aero/sm_car_data_Aero_Coefficients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\Libraries\Vehicle\Aero\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt_srcR22a\Libraries\Vehicle\Aero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FECDE37-2355-42EC-81FD-EEAC9C194360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3575A1AF-0265-4253-9C24-C572FEF119D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11325" tabRatio="760" activeTab="1" xr2:uid="{F771CC24-0E19-4696-9A47-DE53EE9C34AF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="1" xr2:uid="{F771CC24-0E19-4696-9A47-DE53EE9C34AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sedan_HambaLG" sheetId="1" r:id="rId1"/>
@@ -186,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -195,19 +195,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -217,12 +214,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -244,9 +241,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -284,7 +281,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -390,7 +387,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -532,7 +529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -555,7 +552,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
@@ -588,13 +585,13 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -602,103 +599,103 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <v>-0.05</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>1.2250000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
         <v>2.81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>-1.2</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>0</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>0.8</v>
       </c>
     </row>
@@ -720,12 +717,12 @@
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
@@ -758,13 +755,13 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -772,103 +769,103 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <v>-0.05</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <v>0.27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>1.2250000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="14">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13">
         <v>1.98</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>-1.2</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>0</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>0.8</v>
       </c>
     </row>
@@ -895,7 +892,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
@@ -928,13 +925,13 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -942,103 +939,103 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <v>-0.05</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <v>0.43</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>1.2250000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
         <v>2.81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>-1.2</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>0</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>0.8</v>
       </c>
     </row>
@@ -1065,7 +1062,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
@@ -1098,13 +1095,13 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1112,103 +1109,103 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <v>-0.05</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <v>0.43</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>1.2250000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
         <v>2.81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>-1.2</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>0</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -1235,7 +1232,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
@@ -1268,13 +1265,13 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1282,103 +1279,103 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <v>-0.05</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <v>0.27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>1.2250000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
         <v>2.81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>0</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>0</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>1.5</v>
       </c>
     </row>
@@ -1405,7 +1402,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
@@ -1438,13 +1435,13 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1452,103 +1449,103 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <v>-0.05</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <v>0.27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>1.2250000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
         <v>2.81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>1</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>0</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>1.5</v>
       </c>
     </row>
@@ -1575,7 +1572,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
@@ -1608,13 +1605,13 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1622,103 +1619,103 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <v>-0.05</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <v>0.43</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>1.2250000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
         <v>2.81</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>5</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>0</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>2</v>
       </c>
     </row>
@@ -1745,7 +1742,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
@@ -1778,13 +1775,13 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1792,103 +1789,103 @@
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14">
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <v>-2.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14">
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>1.2250000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14">
         <v>1.2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>-0.8</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>0</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>0.6</v>
       </c>
     </row>

</xml_diff>